<commit_message>
added video detection and laptop/home pc detection to set dir
</commit_message>
<xml_diff>
--- a/URLs.xlsx
+++ b/URLs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github local repos\downloader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KP Python\downloader\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -395,11 +395,12 @@
   <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="60.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>

</xml_diff>